<commit_message>
Evaluation of balance created
</commit_message>
<xml_diff>
--- a/V1/Dataset/N2OR.xlsx
+++ b/V1/Dataset/N2OR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\V1\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF10C66-E5E0-4B6D-91A2-5F90CE97B0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED755CD-30A9-4BB3-9DBA-BDC45D6DD1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="22" r:id="rId1"/>
@@ -1737,7 +1737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="196">
   <si>
     <t>Metaheuristics</t>
   </si>
@@ -3092,6 +3092,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3101,12 +3113,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3115,6 +3121,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3128,22 +3140,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3160,6 +3160,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3182,17 +3185,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3561,7 +3561,7 @@
       <c r="E10" s="52"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="60" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="51"/>
@@ -3584,347 +3584,347 @@
       <c r="E13" s="52"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="57"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="57"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="57"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
     </row>
     <row r="27" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="56"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="55"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="56"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="57"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="61"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="34"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="61"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="61"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="43"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="42"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="43"/>
+      <c r="A36" s="62"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="63"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="43"/>
+      <c r="A37" s="62"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="63"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="43"/>
+      <c r="A38" s="62"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="63"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="43"/>
+      <c r="A39" s="62"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="63"/>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="38"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="39"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="43"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="37"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="45"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="32"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="36"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="36"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="32"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="36"/>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="38"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="43"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="39"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="37"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="39"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="41"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="45"/>
     </row>
     <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="60" t="s">
+      <c r="A52" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="60"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="61"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="33"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
       <c r="E53" s="48"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
       <c r="E54" s="48"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="60" t="s">
+      <c r="A55" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="61"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="60" t="s">
+      <c r="A56" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="60"/>
-      <c r="D56" s="60"/>
-      <c r="E56" s="61"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="33"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="29" t="s">
@@ -3933,418 +3933,448 @@
       <c r="E57" s="20"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="32"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="36"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="36"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="44" t="s">
+      <c r="A60" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="44"/>
-      <c r="C60" s="44"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="45"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="44"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="45"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="41"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="44"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="45"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="41"/>
     </row>
     <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="38"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="39"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="43"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="37"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="39"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="36"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="37"/>
+      <c r="A65" s="38"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="39"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="40" t="s">
+      <c r="A66" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="41"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="45"/>
     </row>
     <row r="67" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="60"/>
-      <c r="C67" s="60"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="61"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="46"/>
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="D68" s="46"/>
-      <c r="E68" s="47"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="31"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="37"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="39"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="36"/>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="37"/>
+      <c r="A70" s="38"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="39"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="44" t="s">
+      <c r="A71" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="44"/>
-      <c r="C71" s="44"/>
-      <c r="D71" s="44"/>
-      <c r="E71" s="45"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="41"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="44"/>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="45"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="41"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="44"/>
-      <c r="B73" s="44"/>
-      <c r="C73" s="44"/>
-      <c r="D73" s="44"/>
-      <c r="E73" s="45"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="40"/>
+      <c r="D73" s="40"/>
+      <c r="E73" s="41"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="44"/>
-      <c r="B74" s="44"/>
-      <c r="C74" s="44"/>
-      <c r="D74" s="44"/>
-      <c r="E74" s="45"/>
+      <c r="A74" s="40"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="41"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="44"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="45"/>
+      <c r="A75" s="40"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="41"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="44"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="45"/>
+      <c r="A76" s="40"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="40"/>
+      <c r="D76" s="40"/>
+      <c r="E76" s="41"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="44"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="44"/>
-      <c r="E77" s="45"/>
+      <c r="A77" s="40"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="40"/>
+      <c r="D77" s="40"/>
+      <c r="E77" s="41"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="44"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="45"/>
+      <c r="A78" s="40"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="40"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="41"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="62"/>
-      <c r="B79" s="62"/>
-      <c r="C79" s="62"/>
-      <c r="D79" s="62"/>
-      <c r="E79" s="63"/>
+      <c r="A79" s="46"/>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46"/>
+      <c r="D79" s="46"/>
+      <c r="E79" s="47"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="37"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="39"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="37"/>
+      <c r="A81" s="38"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="39"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="44" t="s">
+      <c r="A82" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="44"/>
-      <c r="C82" s="44"/>
-      <c r="D82" s="44"/>
-      <c r="E82" s="45"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="40"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="41"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="44"/>
-      <c r="B83" s="44"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="45"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="40"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="41"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="44"/>
-      <c r="B84" s="44"/>
-      <c r="C84" s="44"/>
-      <c r="D84" s="44"/>
-      <c r="E84" s="45"/>
+      <c r="A84" s="40"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="40"/>
+      <c r="D84" s="40"/>
+      <c r="E84" s="41"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="44"/>
-      <c r="D85" s="44"/>
-      <c r="E85" s="45"/>
+      <c r="A85" s="40"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="41"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="45"/>
+      <c r="A86" s="40"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="41"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="44"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="44"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="45"/>
+      <c r="A87" s="40"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="41"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="44"/>
-      <c r="B88" s="44"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="45"/>
+      <c r="A88" s="40"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="40"/>
+      <c r="D88" s="40"/>
+      <c r="E88" s="41"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="44"/>
-      <c r="B89" s="44"/>
-      <c r="C89" s="44"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="45"/>
+      <c r="A89" s="40"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="40"/>
+      <c r="D89" s="40"/>
+      <c r="E89" s="41"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="46"/>
-      <c r="B90" s="46"/>
-      <c r="C90" s="46"/>
-      <c r="D90" s="46"/>
-      <c r="E90" s="47"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="31"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="35" t="s">
+      <c r="A91" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="37"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="39"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="36"/>
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="37"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="39"/>
     </row>
     <row r="93" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="44" t="s">
+      <c r="A93" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B93" s="44"/>
-      <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="45"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="40"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="41"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="44"/>
-      <c r="B94" s="44"/>
-      <c r="C94" s="44"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="45"/>
+      <c r="A94" s="40"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="40"/>
+      <c r="D94" s="40"/>
+      <c r="E94" s="41"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="44"/>
-      <c r="B95" s="44"/>
-      <c r="C95" s="44"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="45"/>
+      <c r="A95" s="40"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="40"/>
+      <c r="D95" s="40"/>
+      <c r="E95" s="41"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="44"/>
-      <c r="B96" s="44"/>
-      <c r="C96" s="44"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="45"/>
+      <c r="A96" s="40"/>
+      <c r="B96" s="40"/>
+      <c r="C96" s="40"/>
+      <c r="D96" s="40"/>
+      <c r="E96" s="41"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="44"/>
-      <c r="B97" s="44"/>
-      <c r="C97" s="44"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="45"/>
+      <c r="A97" s="40"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="40"/>
+      <c r="D97" s="40"/>
+      <c r="E97" s="41"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="44"/>
-      <c r="B98" s="44"/>
-      <c r="C98" s="44"/>
-      <c r="D98" s="44"/>
-      <c r="E98" s="45"/>
+      <c r="A98" s="40"/>
+      <c r="B98" s="40"/>
+      <c r="C98" s="40"/>
+      <c r="D98" s="40"/>
+      <c r="E98" s="41"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="44"/>
-      <c r="B99" s="44"/>
-      <c r="C99" s="44"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="45"/>
+      <c r="A99" s="40"/>
+      <c r="B99" s="40"/>
+      <c r="C99" s="40"/>
+      <c r="D99" s="40"/>
+      <c r="E99" s="41"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="44"/>
-      <c r="B100" s="44"/>
-      <c r="C100" s="44"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="45"/>
+      <c r="A100" s="40"/>
+      <c r="B100" s="40"/>
+      <c r="C100" s="40"/>
+      <c r="D100" s="40"/>
+      <c r="E100" s="41"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" s="46"/>
-      <c r="B101" s="46"/>
-      <c r="C101" s="46"/>
-      <c r="D101" s="46"/>
-      <c r="E101" s="47"/>
+      <c r="A101" s="30"/>
+      <c r="B101" s="30"/>
+      <c r="C101" s="30"/>
+      <c r="D101" s="30"/>
+      <c r="E101" s="31"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="35" t="s">
+      <c r="A102" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B102" s="36"/>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="37"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38"/>
+      <c r="E102" s="39"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="36"/>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="37"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="38"/>
+      <c r="E103" s="39"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="44" t="s">
+      <c r="A104" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B104" s="44"/>
-      <c r="C104" s="44"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="45"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="40"/>
+      <c r="D104" s="40"/>
+      <c r="E104" s="41"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="44"/>
-      <c r="B105" s="44"/>
-      <c r="C105" s="44"/>
-      <c r="D105" s="44"/>
-      <c r="E105" s="45"/>
+      <c r="A105" s="40"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="40"/>
+      <c r="D105" s="40"/>
+      <c r="E105" s="41"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="44"/>
-      <c r="B106" s="44"/>
-      <c r="C106" s="44"/>
-      <c r="D106" s="44"/>
-      <c r="E106" s="45"/>
+      <c r="A106" s="40"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="40"/>
+      <c r="D106" s="40"/>
+      <c r="E106" s="41"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="44"/>
-      <c r="B107" s="44"/>
-      <c r="C107" s="44"/>
-      <c r="D107" s="44"/>
-      <c r="E107" s="45"/>
+      <c r="A107" s="40"/>
+      <c r="B107" s="40"/>
+      <c r="C107" s="40"/>
+      <c r="D107" s="40"/>
+      <c r="E107" s="41"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" s="44"/>
-      <c r="B108" s="44"/>
-      <c r="C108" s="44"/>
-      <c r="D108" s="44"/>
-      <c r="E108" s="45"/>
+      <c r="A108" s="40"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="40"/>
+      <c r="D108" s="40"/>
+      <c r="E108" s="41"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" s="44"/>
-      <c r="B109" s="44"/>
-      <c r="C109" s="44"/>
-      <c r="D109" s="44"/>
-      <c r="E109" s="45"/>
+      <c r="A109" s="40"/>
+      <c r="B109" s="40"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="40"/>
+      <c r="E109" s="41"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="44"/>
-      <c r="B110" s="44"/>
-      <c r="C110" s="44"/>
-      <c r="D110" s="44"/>
-      <c r="E110" s="45"/>
+      <c r="A110" s="40"/>
+      <c r="B110" s="40"/>
+      <c r="C110" s="40"/>
+      <c r="D110" s="40"/>
+      <c r="E110" s="41"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" s="44"/>
-      <c r="B111" s="44"/>
-      <c r="C111" s="44"/>
-      <c r="D111" s="44"/>
-      <c r="E111" s="45"/>
+      <c r="A111" s="40"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="40"/>
+      <c r="D111" s="40"/>
+      <c r="E111" s="41"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="46"/>
-      <c r="B112" s="46"/>
-      <c r="C112" s="46"/>
-      <c r="D112" s="46"/>
-      <c r="E112" s="47"/>
+      <c r="A112" s="30"/>
+      <c r="B112" s="30"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A44:E45"/>
+    <mergeCell ref="A46:E47"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A41:E42"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E39"/>
+    <mergeCell ref="A80:E81"/>
+    <mergeCell ref="A82:E89"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A53:E54"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A4:E10"/>
+    <mergeCell ref="A15:E16"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A17:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="A24:E26"/>
+    <mergeCell ref="A11:E13"/>
+    <mergeCell ref="A20:E21"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A27:E29"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A79:E79"/>
     <mergeCell ref="A112:E112"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A58:E59"/>
@@ -4361,36 +4391,6 @@
     <mergeCell ref="A71:E78"/>
     <mergeCell ref="A102:E103"/>
     <mergeCell ref="A104:E111"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A80:E81"/>
-    <mergeCell ref="A82:E89"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A53:E54"/>
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A4:E10"/>
-    <mergeCell ref="A15:E16"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A17:E18"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A22:E23"/>
-    <mergeCell ref="A24:E26"/>
-    <mergeCell ref="A11:E13"/>
-    <mergeCell ref="A20:E21"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A27:E29"/>
-    <mergeCell ref="A44:E45"/>
-    <mergeCell ref="A46:E47"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A41:E42"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4562,7 +4562,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
@@ -4639,7 +4639,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4760,7 +4760,7 @@
         <v>158</v>
       </c>
       <c r="E10" s="27">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -4943,9 +4943,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T157"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7026,7 +7026,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7069,144 +7069,249 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>161</v>
+      </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>164</v>
+      </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>165</v>
+      </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>167</v>
+      </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>168</v>
+      </c>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>169</v>
+      </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>177</v>
+      </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>178</v>
+      </c>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>181</v>
+      </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>182</v>
+      </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>183</v>
+      </c>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>184</v>
+      </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>189</v>
+      </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>190</v>
+      </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>191</v>
+      </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>192</v>
+      </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>194</v>
+      </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.3">
@@ -7237,7 +7342,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>